<commit_message>
working but with error
some doubt in cal
</commit_message>
<xml_diff>
--- a/AprajitaRetails/Server/wwwroot/Data/SaleData2023.xlsx
+++ b/AprajitaRetails/Server/wwwroot/Data/SaleData2023.xlsx
@@ -1824,12 +1824,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1846,16 +1846,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1864,111 +1857,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1990,10 +1878,115 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2018,13 +2011,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2036,7 +2119,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2048,25 +2143,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2078,13 +2161,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2096,109 +2179,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2295,6 +2288,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2336,20 +2340,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2369,6 +2362,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2383,160 +2385,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2673,7 +2666,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:L689" totalsRowCount="1">
-  <autoFilter ref="A1:L688"/>
+  <autoFilter ref="A1:L688">
+    <filterColumn colId="1">
+      <filters>
+        <dateGroupItem year="2023" month="2" dateTimeGrouping="month"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="12">
     <tableColumn id="1" name="SN" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Date" dataDxfId="0"/>
@@ -14032,7 +14031,7 @@
   <dimension ref="A1:L689"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -18144,7 +18143,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="111" spans="1:12">
+    <row r="111" hidden="1" spans="1:12">
       <c r="A111">
         <v>110</v>
       </c>
@@ -18182,7 +18181,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" hidden="1" spans="1:11">
       <c r="A112">
         <v>111</v>
       </c>
@@ -18217,7 +18216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:12">
+    <row r="113" hidden="1" spans="1:12">
       <c r="A113">
         <v>112</v>
       </c>
@@ -18255,7 +18254,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" hidden="1" spans="1:12">
       <c r="A114">
         <v>113</v>
       </c>
@@ -18293,7 +18292,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" hidden="1" spans="1:12">
       <c r="A115">
         <v>114</v>
       </c>
@@ -18331,7 +18330,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" hidden="1" spans="1:12">
       <c r="A116">
         <v>115</v>
       </c>
@@ -18369,7 +18368,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" hidden="1" spans="1:12">
       <c r="A117">
         <v>116</v>
       </c>
@@ -18407,7 +18406,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="118" spans="1:12">
+    <row r="118" hidden="1" spans="1:12">
       <c r="A118">
         <v>117</v>
       </c>
@@ -18445,7 +18444,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" hidden="1" spans="1:12">
       <c r="A119">
         <v>118</v>
       </c>
@@ -18483,7 +18482,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" hidden="1" spans="1:12">
       <c r="A120">
         <v>119</v>
       </c>
@@ -18521,7 +18520,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" hidden="1" spans="1:12">
       <c r="A121">
         <v>120</v>
       </c>
@@ -18559,7 +18558,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" hidden="1" spans="1:11">
       <c r="A122">
         <v>121</v>
       </c>
@@ -18594,7 +18593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" hidden="1" spans="1:12">
       <c r="A123">
         <v>122</v>
       </c>
@@ -18632,7 +18631,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" hidden="1" spans="1:12">
       <c r="A124">
         <v>123</v>
       </c>
@@ -18670,7 +18669,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" hidden="1" spans="1:12">
       <c r="A125">
         <v>124</v>
       </c>
@@ -18708,7 +18707,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" hidden="1" spans="1:12">
       <c r="A126">
         <v>125</v>
       </c>
@@ -18746,7 +18745,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="127" spans="1:12">
+    <row r="127" hidden="1" spans="1:12">
       <c r="A127">
         <v>126</v>
       </c>
@@ -18784,7 +18783,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="128" spans="1:12">
+    <row r="128" hidden="1" spans="1:12">
       <c r="A128">
         <v>127</v>
       </c>
@@ -18822,7 +18821,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="129" spans="1:12">
+    <row r="129" hidden="1" spans="1:12">
       <c r="A129">
         <v>128</v>
       </c>
@@ -18860,7 +18859,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="130" spans="1:12">
+    <row r="130" hidden="1" spans="1:12">
       <c r="A130">
         <v>129</v>
       </c>
@@ -18898,7 +18897,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="131" spans="1:12">
+    <row r="131" hidden="1" spans="1:12">
       <c r="A131">
         <v>130</v>
       </c>
@@ -18936,7 +18935,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
+    <row r="132" hidden="1" spans="1:11">
       <c r="A132">
         <v>131</v>
       </c>
@@ -18971,7 +18970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
+    <row r="133" hidden="1" spans="1:11">
       <c r="A133">
         <v>132</v>
       </c>
@@ -19006,7 +19005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" hidden="1" spans="1:11">
       <c r="A134">
         <v>133</v>
       </c>
@@ -19041,7 +19040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11">
+    <row r="135" hidden="1" spans="1:11">
       <c r="A135">
         <v>134</v>
       </c>
@@ -19076,7 +19075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11">
+    <row r="136" hidden="1" spans="1:11">
       <c r="A136">
         <v>135</v>
       </c>
@@ -19111,7 +19110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:11">
+    <row r="137" hidden="1" spans="1:11">
       <c r="A137">
         <v>136</v>
       </c>
@@ -19146,7 +19145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:12">
+    <row r="138" hidden="1" spans="1:12">
       <c r="A138">
         <v>137</v>
       </c>
@@ -19184,7 +19183,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="139" spans="1:11">
+    <row r="139" hidden="1" spans="1:11">
       <c r="A139">
         <v>138</v>
       </c>
@@ -19219,7 +19218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12">
+    <row r="140" hidden="1" spans="1:12">
       <c r="A140">
         <v>139</v>
       </c>
@@ -19257,7 +19256,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="141" spans="1:12">
+    <row r="141" hidden="1" spans="1:12">
       <c r="A141">
         <v>140</v>
       </c>
@@ -19295,7 +19294,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="142" spans="1:12">
+    <row r="142" hidden="1" spans="1:12">
       <c r="A142">
         <v>141</v>
       </c>
@@ -19333,7 +19332,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="143" spans="1:12">
+    <row r="143" hidden="1" spans="1:12">
       <c r="A143">
         <v>142</v>
       </c>
@@ -19371,7 +19370,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="144" spans="1:12">
+    <row r="144" hidden="1" spans="1:12">
       <c r="A144">
         <v>143</v>
       </c>
@@ -19409,7 +19408,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="145" spans="1:12">
+    <row r="145" hidden="1" spans="1:12">
       <c r="A145">
         <v>144</v>
       </c>
@@ -19447,7 +19446,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="146" spans="1:11">
+    <row r="146" hidden="1" spans="1:11">
       <c r="A146">
         <v>145</v>
       </c>
@@ -19482,7 +19481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:12">
+    <row r="147" hidden="1" spans="1:12">
       <c r="A147">
         <v>146</v>
       </c>
@@ -19520,7 +19519,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="148" spans="1:12">
+    <row r="148" hidden="1" spans="1:12">
       <c r="A148">
         <v>147</v>
       </c>
@@ -19558,7 +19557,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="149" spans="1:12">
+    <row r="149" hidden="1" spans="1:12">
       <c r="A149">
         <v>148</v>
       </c>
@@ -19596,7 +19595,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="150" spans="1:12">
+    <row r="150" hidden="1" spans="1:12">
       <c r="A150">
         <v>149</v>
       </c>
@@ -19634,7 +19633,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="151" spans="1:12">
+    <row r="151" hidden="1" spans="1:12">
       <c r="A151">
         <v>150</v>
       </c>
@@ -19672,7 +19671,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="152" spans="1:12">
+    <row r="152" hidden="1" spans="1:12">
       <c r="A152">
         <v>151</v>
       </c>
@@ -19710,7 +19709,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="153" spans="1:12">
+    <row r="153" hidden="1" spans="1:12">
       <c r="A153">
         <v>152</v>
       </c>
@@ -19748,7 +19747,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="154" spans="1:12">
+    <row r="154" hidden="1" spans="1:12">
       <c r="A154">
         <v>153</v>
       </c>
@@ -19786,7 +19785,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="155" spans="1:12">
+    <row r="155" hidden="1" spans="1:12">
       <c r="A155">
         <v>154</v>
       </c>
@@ -19824,7 +19823,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="156" spans="1:12">
+    <row r="156" hidden="1" spans="1:12">
       <c r="A156">
         <v>155</v>
       </c>
@@ -19862,7 +19861,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="157" spans="1:12">
+    <row r="157" hidden="1" spans="1:12">
       <c r="A157">
         <v>156</v>
       </c>
@@ -19900,7 +19899,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="158" spans="1:12">
+    <row r="158" hidden="1" spans="1:12">
       <c r="A158">
         <v>157</v>
       </c>
@@ -19938,7 +19937,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="159" spans="1:11">
+    <row r="159" hidden="1" spans="1:11">
       <c r="A159">
         <v>158</v>
       </c>
@@ -19973,7 +19972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:11">
+    <row r="160" hidden="1" spans="1:11">
       <c r="A160">
         <v>159</v>
       </c>
@@ -20008,7 +20007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:11">
+    <row r="161" hidden="1" spans="1:11">
       <c r="A161">
         <v>160</v>
       </c>
@@ -20043,7 +20042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:12">
+    <row r="162" hidden="1" spans="1:12">
       <c r="A162">
         <v>161</v>
       </c>
@@ -20081,7 +20080,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="163" spans="1:12">
+    <row r="163" hidden="1" spans="1:12">
       <c r="A163">
         <v>162</v>
       </c>
@@ -20119,7 +20118,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="164" spans="1:12">
+    <row r="164" hidden="1" spans="1:12">
       <c r="A164">
         <v>163</v>
       </c>
@@ -20157,7 +20156,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="165" spans="1:12">
+    <row r="165" hidden="1" spans="1:12">
       <c r="A165">
         <v>164</v>
       </c>
@@ -20195,7 +20194,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="166" spans="1:12">
+    <row r="166" hidden="1" spans="1:12">
       <c r="A166">
         <v>165</v>
       </c>
@@ -20233,7 +20232,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="167" spans="1:11">
+    <row r="167" hidden="1" spans="1:11">
       <c r="A167">
         <v>166</v>
       </c>
@@ -20268,7 +20267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:12">
+    <row r="168" hidden="1" spans="1:12">
       <c r="A168">
         <v>167</v>
       </c>
@@ -20306,7 +20305,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="169" spans="1:12">
+    <row r="169" hidden="1" spans="1:12">
       <c r="A169">
         <v>168</v>
       </c>
@@ -20344,7 +20343,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="170" spans="1:12">
+    <row r="170" hidden="1" spans="1:12">
       <c r="A170">
         <v>169</v>
       </c>
@@ -20382,7 +20381,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="171" spans="1:12">
+    <row r="171" hidden="1" spans="1:12">
       <c r="A171">
         <v>170</v>
       </c>
@@ -20420,7 +20419,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="172" spans="1:12">
+    <row r="172" hidden="1" spans="1:12">
       <c r="A172">
         <v>171</v>
       </c>
@@ -20458,7 +20457,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="173" spans="1:12">
+    <row r="173" hidden="1" spans="1:12">
       <c r="A173">
         <v>172</v>
       </c>
@@ -20496,7 +20495,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="174" spans="1:12">
+    <row r="174" hidden="1" spans="1:12">
       <c r="A174">
         <v>173</v>
       </c>
@@ -20534,7 +20533,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="175" spans="1:12">
+    <row r="175" hidden="1" spans="1:12">
       <c r="A175">
         <v>174</v>
       </c>
@@ -20572,7 +20571,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="176" spans="1:12">
+    <row r="176" hidden="1" spans="1:12">
       <c r="A176">
         <v>175</v>
       </c>
@@ -20610,7 +20609,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="177" spans="1:12">
+    <row r="177" hidden="1" spans="1:12">
       <c r="A177">
         <v>176</v>
       </c>
@@ -20648,7 +20647,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="178" spans="1:12">
+    <row r="178" hidden="1" spans="1:12">
       <c r="A178">
         <v>177</v>
       </c>
@@ -20686,7 +20685,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="179" spans="1:12">
+    <row r="179" hidden="1" spans="1:12">
       <c r="A179">
         <v>178</v>
       </c>
@@ -20724,7 +20723,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="180" spans="1:12">
+    <row r="180" hidden="1" spans="1:12">
       <c r="A180">
         <v>179</v>
       </c>
@@ -20762,7 +20761,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="181" spans="1:12">
+    <row r="181" hidden="1" spans="1:12">
       <c r="A181">
         <v>180</v>
       </c>
@@ -20800,7 +20799,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="182" spans="1:11">
+    <row r="182" hidden="1" spans="1:11">
       <c r="A182">
         <v>181</v>
       </c>
@@ -20835,7 +20834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:12">
+    <row r="183" hidden="1" spans="1:12">
       <c r="A183">
         <v>182</v>
       </c>
@@ -20873,7 +20872,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="184" spans="1:12">
+    <row r="184" hidden="1" spans="1:12">
       <c r="A184">
         <v>183</v>
       </c>
@@ -20911,7 +20910,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="185" spans="1:12">
+    <row r="185" hidden="1" spans="1:12">
       <c r="A185">
         <v>184</v>
       </c>
@@ -20949,7 +20948,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="186" spans="1:12">
+    <row r="186" hidden="1" spans="1:12">
       <c r="A186">
         <v>185</v>
       </c>
@@ -20987,7 +20986,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="187" spans="1:12">
+    <row r="187" hidden="1" spans="1:12">
       <c r="A187">
         <v>186</v>
       </c>
@@ -21025,7 +21024,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="188" spans="1:12">
+    <row r="188" hidden="1" spans="1:12">
       <c r="A188">
         <v>187</v>
       </c>
@@ -21063,7 +21062,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="189" spans="1:12">
+    <row r="189" hidden="1" spans="1:12">
       <c r="A189">
         <v>188</v>
       </c>
@@ -21101,7 +21100,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="190" spans="1:12">
+    <row r="190" hidden="1" spans="1:12">
       <c r="A190">
         <v>189</v>
       </c>
@@ -21139,7 +21138,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="191" spans="1:11">
+    <row r="191" hidden="1" spans="1:11">
       <c r="A191">
         <v>190</v>
       </c>
@@ -21174,7 +21173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:11">
+    <row r="192" hidden="1" spans="1:11">
       <c r="A192">
         <v>191</v>
       </c>
@@ -21209,7 +21208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:11">
+    <row r="193" hidden="1" spans="1:11">
       <c r="A193">
         <v>192</v>
       </c>
@@ -21244,7 +21243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:12">
+    <row r="194" hidden="1" spans="1:12">
       <c r="A194">
         <v>193</v>
       </c>
@@ -21282,7 +21281,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="195" spans="1:12">
+    <row r="195" hidden="1" spans="1:12">
       <c r="A195">
         <v>194</v>
       </c>
@@ -21320,7 +21319,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="196" spans="1:12">
+    <row r="196" hidden="1" spans="1:12">
       <c r="A196">
         <v>195</v>
       </c>
@@ -21358,7 +21357,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="197" spans="1:12">
+    <row r="197" hidden="1" spans="1:12">
       <c r="A197">
         <v>196</v>
       </c>
@@ -21396,7 +21395,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="198" spans="1:12">
+    <row r="198" hidden="1" spans="1:12">
       <c r="A198">
         <v>197</v>
       </c>
@@ -21434,7 +21433,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="199" spans="1:12">
+    <row r="199" hidden="1" spans="1:12">
       <c r="A199">
         <v>198</v>
       </c>
@@ -21472,7 +21471,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="200" spans="1:12">
+    <row r="200" hidden="1" spans="1:12">
       <c r="A200">
         <v>199</v>
       </c>
@@ -21510,7 +21509,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="201" spans="1:11">
+    <row r="201" hidden="1" spans="1:11">
       <c r="A201">
         <v>200</v>
       </c>
@@ -21545,7 +21544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:11">
+    <row r="202" hidden="1" spans="1:11">
       <c r="A202">
         <v>201</v>
       </c>
@@ -21580,7 +21579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:11">
+    <row r="203" hidden="1" spans="1:11">
       <c r="A203">
         <v>202</v>
       </c>
@@ -21615,7 +21614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:12">
+    <row r="204" hidden="1" spans="1:12">
       <c r="A204">
         <v>203</v>
       </c>
@@ -21653,7 +21652,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="205" spans="1:11">
+    <row r="205" hidden="1" spans="1:11">
       <c r="A205">
         <v>204</v>
       </c>
@@ -21688,7 +21687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:11">
+    <row r="206" hidden="1" spans="1:11">
       <c r="A206">
         <v>205</v>
       </c>
@@ -21723,7 +21722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:12">
+    <row r="207" hidden="1" spans="1:12">
       <c r="A207">
         <v>206</v>
       </c>
@@ -21761,7 +21760,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="208" spans="1:12">
+    <row r="208" hidden="1" spans="1:12">
       <c r="A208">
         <v>207</v>
       </c>
@@ -21799,7 +21798,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="209" spans="1:12">
+    <row r="209" hidden="1" spans="1:12">
       <c r="A209">
         <v>208</v>
       </c>
@@ -21837,7 +21836,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="210" spans="1:12">
+    <row r="210" hidden="1" spans="1:12">
       <c r="A210">
         <v>209</v>
       </c>
@@ -21875,7 +21874,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="211" spans="1:12">
+    <row r="211" hidden="1" spans="1:12">
       <c r="A211">
         <v>210</v>
       </c>
@@ -21913,7 +21912,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="212" spans="1:12">
+    <row r="212" hidden="1" spans="1:12">
       <c r="A212">
         <v>211</v>
       </c>
@@ -21951,7 +21950,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="213" spans="1:12">
+    <row r="213" hidden="1" spans="1:12">
       <c r="A213">
         <v>212</v>
       </c>
@@ -21989,7 +21988,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="214" spans="1:12">
+    <row r="214" hidden="1" spans="1:12">
       <c r="A214">
         <v>213</v>
       </c>
@@ -22027,7 +22026,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="215" spans="1:12">
+    <row r="215" hidden="1" spans="1:12">
       <c r="A215">
         <v>214</v>
       </c>
@@ -22065,7 +22064,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="216" spans="1:12">
+    <row r="216" hidden="1" spans="1:12">
       <c r="A216">
         <v>215</v>
       </c>
@@ -22103,7 +22102,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="217" spans="1:12">
+    <row r="217" hidden="1" spans="1:12">
       <c r="A217">
         <v>216</v>
       </c>
@@ -22141,7 +22140,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="218" spans="1:12">
+    <row r="218" hidden="1" spans="1:12">
       <c r="A218">
         <v>217</v>
       </c>
@@ -22179,7 +22178,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="219" spans="1:12">
+    <row r="219" hidden="1" spans="1:12">
       <c r="A219">
         <v>218</v>
       </c>
@@ -22217,7 +22216,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="220" spans="1:12">
+    <row r="220" hidden="1" spans="1:12">
       <c r="A220">
         <v>219</v>
       </c>
@@ -22255,7 +22254,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="221" spans="1:12">
+    <row r="221" hidden="1" spans="1:12">
       <c r="A221">
         <v>220</v>
       </c>
@@ -22293,7 +22292,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="222" spans="1:12">
+    <row r="222" hidden="1" spans="1:12">
       <c r="A222">
         <v>221</v>
       </c>
@@ -22331,7 +22330,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="223" spans="1:12">
+    <row r="223" hidden="1" spans="1:12">
       <c r="A223">
         <v>222</v>
       </c>
@@ -22369,7 +22368,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="224" spans="1:12">
+    <row r="224" hidden="1" spans="1:12">
       <c r="A224">
         <v>223</v>
       </c>
@@ -22407,7 +22406,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="225" spans="1:11">
+    <row r="225" hidden="1" spans="1:11">
       <c r="A225">
         <v>224</v>
       </c>
@@ -22442,7 +22441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:11">
+    <row r="226" hidden="1" spans="1:11">
       <c r="A226">
         <v>225</v>
       </c>
@@ -22477,7 +22476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:11">
+    <row r="227" hidden="1" spans="1:11">
       <c r="A227">
         <v>226</v>
       </c>
@@ -22512,7 +22511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:11">
+    <row r="228" hidden="1" spans="1:11">
       <c r="A228">
         <v>227</v>
       </c>
@@ -22547,7 +22546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:12">
+    <row r="229" hidden="1" spans="1:12">
       <c r="A229">
         <v>228</v>
       </c>
@@ -22585,7 +22584,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="230" spans="1:12">
+    <row r="230" hidden="1" spans="1:12">
       <c r="A230">
         <v>229</v>
       </c>
@@ -22623,7 +22622,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="231" spans="1:12">
+    <row r="231" hidden="1" spans="1:12">
       <c r="A231">
         <v>230</v>
       </c>
@@ -22661,7 +22660,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="232" spans="1:12">
+    <row r="232" hidden="1" spans="1:12">
       <c r="A232">
         <v>231</v>
       </c>
@@ -22699,7 +22698,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="233" spans="1:12">
+    <row r="233" hidden="1" spans="1:12">
       <c r="A233">
         <v>232</v>
       </c>
@@ -22737,7 +22736,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="234" spans="1:12">
+    <row r="234" hidden="1" spans="1:12">
       <c r="A234">
         <v>233</v>
       </c>
@@ -22775,7 +22774,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="235" spans="1:11">
+    <row r="235" hidden="1" spans="1:11">
       <c r="A235">
         <v>234</v>
       </c>
@@ -22810,7 +22809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:12">
+    <row r="236" hidden="1" spans="1:12">
       <c r="A236">
         <v>235</v>
       </c>
@@ -22848,7 +22847,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="237" spans="1:12">
+    <row r="237" hidden="1" spans="1:12">
       <c r="A237">
         <v>236</v>
       </c>
@@ -22886,7 +22885,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="238" spans="1:12">
+    <row r="238" hidden="1" spans="1:12">
       <c r="A238">
         <v>237</v>
       </c>
@@ -22924,7 +22923,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="239" spans="1:12">
+    <row r="239" hidden="1" spans="1:12">
       <c r="A239">
         <v>238</v>
       </c>
@@ -22962,7 +22961,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="240" spans="1:12">
+    <row r="240" hidden="1" spans="1:12">
       <c r="A240">
         <v>239</v>
       </c>
@@ -23000,7 +22999,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="241" spans="1:12">
+    <row r="241" hidden="1" spans="1:12">
       <c r="A241">
         <v>240</v>
       </c>
@@ -23038,7 +23037,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="242" spans="1:12">
+    <row r="242" hidden="1" spans="1:12">
       <c r="A242">
         <v>241</v>
       </c>
@@ -23076,7 +23075,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="243" spans="1:12">
+    <row r="243" hidden="1" spans="1:12">
       <c r="A243">
         <v>242</v>
       </c>
@@ -23114,7 +23113,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="244" spans="1:12">
+    <row r="244" hidden="1" spans="1:12">
       <c r="A244">
         <v>243</v>
       </c>
@@ -23152,7 +23151,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="245" spans="1:12">
+    <row r="245" hidden="1" spans="1:12">
       <c r="A245">
         <v>244</v>
       </c>
@@ -23190,7 +23189,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="246" spans="1:12">
+    <row r="246" hidden="1" spans="1:12">
       <c r="A246">
         <v>245</v>
       </c>
@@ -23228,7 +23227,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="247" spans="1:12">
+    <row r="247" hidden="1" spans="1:12">
       <c r="A247">
         <v>246</v>
       </c>
@@ -23266,7 +23265,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="248" spans="1:12">
+    <row r="248" hidden="1" spans="1:12">
       <c r="A248">
         <v>247</v>
       </c>
@@ -23304,7 +23303,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="249" spans="1:12">
+    <row r="249" hidden="1" spans="1:12">
       <c r="A249">
         <v>248</v>
       </c>
@@ -23342,7 +23341,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="250" spans="1:12">
+    <row r="250" hidden="1" spans="1:12">
       <c r="A250">
         <v>249</v>
       </c>
@@ -23380,7 +23379,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="251" spans="1:12">
+    <row r="251" hidden="1" spans="1:12">
       <c r="A251">
         <v>250</v>
       </c>
@@ -23418,7 +23417,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="252" spans="1:12">
+    <row r="252" hidden="1" spans="1:12">
       <c r="A252">
         <v>251</v>
       </c>
@@ -23456,7 +23455,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="253" spans="1:12">
+    <row r="253" hidden="1" spans="1:12">
       <c r="A253">
         <v>252</v>
       </c>
@@ -23494,7 +23493,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="254" spans="1:12">
+    <row r="254" hidden="1" spans="1:12">
       <c r="A254">
         <v>253</v>
       </c>
@@ -23532,7 +23531,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="255" spans="1:12">
+    <row r="255" hidden="1" spans="1:12">
       <c r="A255">
         <v>254</v>
       </c>
@@ -23570,7 +23569,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="256" spans="1:12">
+    <row r="256" hidden="1" spans="1:12">
       <c r="A256">
         <v>255</v>
       </c>
@@ -23608,7 +23607,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="257" spans="1:12">
+    <row r="257" hidden="1" spans="1:12">
       <c r="A257">
         <v>256</v>
       </c>
@@ -23646,7 +23645,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="258" spans="1:12">
+    <row r="258" hidden="1" spans="1:12">
       <c r="A258">
         <v>257</v>
       </c>
@@ -23684,7 +23683,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="259" spans="1:12">
+    <row r="259" hidden="1" spans="1:12">
       <c r="A259">
         <v>258</v>
       </c>
@@ -23722,7 +23721,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="260" spans="1:12">
+    <row r="260" hidden="1" spans="1:12">
       <c r="A260">
         <v>259</v>
       </c>
@@ -23760,7 +23759,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="261" spans="1:12">
+    <row r="261" hidden="1" spans="1:12">
       <c r="A261">
         <v>260</v>
       </c>
@@ -23798,7 +23797,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="262" spans="1:12">
+    <row r="262" hidden="1" spans="1:12">
       <c r="A262">
         <v>261</v>
       </c>
@@ -23836,7 +23835,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="263" spans="1:11">
+    <row r="263" hidden="1" spans="1:11">
       <c r="A263">
         <v>262</v>
       </c>
@@ -23871,7 +23870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:11">
+    <row r="264" hidden="1" spans="1:11">
       <c r="A264">
         <v>263</v>
       </c>
@@ -23906,7 +23905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:12">
+    <row r="265" hidden="1" spans="1:12">
       <c r="A265">
         <v>264</v>
       </c>
@@ -23944,7 +23943,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="266" spans="1:12">
+    <row r="266" hidden="1" spans="1:12">
       <c r="A266">
         <v>265</v>
       </c>
@@ -23982,7 +23981,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="267" spans="1:12">
+    <row r="267" hidden="1" spans="1:12">
       <c r="A267">
         <v>266</v>
       </c>
@@ -24020,7 +24019,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="268" spans="1:12">
+    <row r="268" hidden="1" spans="1:12">
       <c r="A268">
         <v>267</v>
       </c>
@@ -24058,7 +24057,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="269" spans="1:12">
+    <row r="269" hidden="1" spans="1:12">
       <c r="A269">
         <v>268</v>
       </c>
@@ -24096,7 +24095,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="270" spans="1:12">
+    <row r="270" hidden="1" spans="1:12">
       <c r="A270">
         <v>269</v>
       </c>
@@ -24134,7 +24133,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="271" spans="1:12">
+    <row r="271" hidden="1" spans="1:12">
       <c r="A271">
         <v>270</v>
       </c>
@@ -24172,7 +24171,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="272" spans="1:11">
+    <row r="272" hidden="1" spans="1:11">
       <c r="A272">
         <v>271</v>
       </c>
@@ -24207,7 +24206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:11">
+    <row r="273" hidden="1" spans="1:11">
       <c r="A273">
         <v>272</v>
       </c>
@@ -24242,7 +24241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:11">
+    <row r="274" hidden="1" spans="1:11">
       <c r="A274">
         <v>273</v>
       </c>
@@ -24277,7 +24276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:12">
+    <row r="275" hidden="1" spans="1:12">
       <c r="A275">
         <v>274</v>
       </c>
@@ -24315,7 +24314,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="276" spans="1:12">
+    <row r="276" hidden="1" spans="1:12">
       <c r="A276">
         <v>275</v>
       </c>
@@ -24353,7 +24352,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="277" spans="1:12">
+    <row r="277" hidden="1" spans="1:12">
       <c r="A277">
         <v>276</v>
       </c>
@@ -24391,7 +24390,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="278" spans="1:12">
+    <row r="278" hidden="1" spans="1:12">
       <c r="A278">
         <v>277</v>
       </c>
@@ -24429,7 +24428,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="279" spans="1:12">
+    <row r="279" hidden="1" spans="1:12">
       <c r="A279">
         <v>278</v>
       </c>
@@ -24467,7 +24466,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="280" spans="1:12">
+    <row r="280" hidden="1" spans="1:12">
       <c r="A280">
         <v>279</v>
       </c>
@@ -24505,7 +24504,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="281" spans="1:12">
+    <row r="281" hidden="1" spans="1:12">
       <c r="A281">
         <v>280</v>
       </c>
@@ -24543,7 +24542,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="282" spans="1:12">
+    <row r="282" hidden="1" spans="1:12">
       <c r="A282">
         <v>281</v>
       </c>
@@ -24581,7 +24580,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="283" spans="1:12">
+    <row r="283" hidden="1" spans="1:12">
       <c r="A283">
         <v>282</v>
       </c>
@@ -24619,7 +24618,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="284" spans="1:12">
+    <row r="284" hidden="1" spans="1:12">
       <c r="A284">
         <v>283</v>
       </c>
@@ -24657,7 +24656,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="285" spans="1:11">
+    <row r="285" hidden="1" spans="1:11">
       <c r="A285">
         <v>284</v>
       </c>
@@ -24692,7 +24691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:11">
+    <row r="286" hidden="1" spans="1:11">
       <c r="A286">
         <v>285</v>
       </c>
@@ -24727,7 +24726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:12">
+    <row r="287" hidden="1" spans="1:12">
       <c r="A287">
         <v>286</v>
       </c>
@@ -24765,7 +24764,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="288" spans="1:12">
+    <row r="288" hidden="1" spans="1:12">
       <c r="A288">
         <v>287</v>
       </c>
@@ -24803,7 +24802,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="289" spans="1:12">
+    <row r="289" hidden="1" spans="1:12">
       <c r="A289">
         <v>288</v>
       </c>
@@ -24841,7 +24840,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="290" spans="1:12">
+    <row r="290" hidden="1" spans="1:12">
       <c r="A290">
         <v>289</v>
       </c>
@@ -24879,7 +24878,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="291" spans="1:12">
+    <row r="291" hidden="1" spans="1:12">
       <c r="A291">
         <v>290</v>
       </c>
@@ -24917,7 +24916,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="292" spans="1:12">
+    <row r="292" hidden="1" spans="1:12">
       <c r="A292">
         <v>291</v>
       </c>
@@ -24955,7 +24954,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="293" spans="1:11">
+    <row r="293" hidden="1" spans="1:11">
       <c r="A293">
         <v>292</v>
       </c>
@@ -24990,7 +24989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:11">
+    <row r="294" hidden="1" spans="1:11">
       <c r="A294">
         <v>293</v>
       </c>
@@ -25025,7 +25024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:11">
+    <row r="295" hidden="1" spans="1:11">
       <c r="A295">
         <v>294</v>
       </c>
@@ -25060,7 +25059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:11">
+    <row r="296" hidden="1" spans="1:11">
       <c r="A296">
         <v>295</v>
       </c>
@@ -25095,7 +25094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:12">
+    <row r="297" hidden="1" spans="1:12">
       <c r="A297">
         <v>296</v>
       </c>
@@ -25133,7 +25132,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="298" spans="1:12">
+    <row r="298" hidden="1" spans="1:12">
       <c r="A298">
         <v>297</v>
       </c>
@@ -25171,7 +25170,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="299" spans="1:12">
+    <row r="299" hidden="1" spans="1:12">
       <c r="A299">
         <v>298</v>
       </c>
@@ -25209,7 +25208,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="300" spans="1:12">
+    <row r="300" hidden="1" spans="1:12">
       <c r="A300">
         <v>299</v>
       </c>
@@ -25247,7 +25246,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="301" spans="1:12">
+    <row r="301" hidden="1" spans="1:12">
       <c r="A301">
         <v>300</v>
       </c>
@@ -25285,7 +25284,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="302" spans="1:12">
+    <row r="302" hidden="1" spans="1:12">
       <c r="A302">
         <v>301</v>
       </c>
@@ -25323,7 +25322,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="303" spans="1:11">
+    <row r="303" hidden="1" spans="1:11">
       <c r="A303">
         <v>302</v>
       </c>
@@ -25358,7 +25357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:11">
+    <row r="304" hidden="1" spans="1:11">
       <c r="A304">
         <v>303</v>
       </c>
@@ -25393,7 +25392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:11">
+    <row r="305" hidden="1" spans="1:11">
       <c r="A305">
         <v>304</v>
       </c>
@@ -25428,7 +25427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:11">
+    <row r="306" hidden="1" spans="1:11">
       <c r="A306">
         <v>305</v>
       </c>
@@ -25463,7 +25462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:11">
+    <row r="307" hidden="1" spans="1:11">
       <c r="A307">
         <v>306</v>
       </c>
@@ -25498,7 +25497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:11">
+    <row r="308" hidden="1" spans="1:11">
       <c r="A308">
         <v>307</v>
       </c>
@@ -25533,7 +25532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:12">
+    <row r="309" hidden="1" spans="1:12">
       <c r="A309">
         <v>308</v>
       </c>
@@ -25571,7 +25570,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="310" spans="1:11">
+    <row r="310" hidden="1" spans="1:11">
       <c r="A310">
         <v>309</v>
       </c>
@@ -25606,7 +25605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:11">
+    <row r="311" hidden="1" spans="1:11">
       <c r="A311">
         <v>310</v>
       </c>
@@ -25641,7 +25640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:11">
+    <row r="312" hidden="1" spans="1:11">
       <c r="A312">
         <v>311</v>
       </c>
@@ -25676,7 +25675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:11">
+    <row r="313" hidden="1" spans="1:11">
       <c r="A313">
         <v>312</v>
       </c>
@@ -25711,7 +25710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:11">
+    <row r="314" hidden="1" spans="1:11">
       <c r="A314">
         <v>313</v>
       </c>
@@ -25746,7 +25745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:11">
+    <row r="315" hidden="1" spans="1:11">
       <c r="A315">
         <v>314</v>
       </c>
@@ -25781,7 +25780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:11">
+    <row r="316" hidden="1" spans="1:11">
       <c r="A316">
         <v>315</v>
       </c>
@@ -25816,7 +25815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:11">
+    <row r="317" hidden="1" spans="1:11">
       <c r="A317">
         <v>316</v>
       </c>
@@ -25851,7 +25850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:11">
+    <row r="318" hidden="1" spans="1:11">
       <c r="A318">
         <v>317</v>
       </c>
@@ -25886,7 +25885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:11">
+    <row r="319" hidden="1" spans="1:11">
       <c r="A319">
         <v>318</v>
       </c>
@@ -25921,7 +25920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:11">
+    <row r="320" hidden="1" spans="1:11">
       <c r="A320">
         <v>319</v>
       </c>
@@ -25956,7 +25955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:11">
+    <row r="321" hidden="1" spans="1:11">
       <c r="A321">
         <v>320</v>
       </c>
@@ -25991,7 +25990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:11">
+    <row r="322" hidden="1" spans="1:11">
       <c r="A322">
         <v>321</v>
       </c>
@@ -26026,7 +26025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:12">
+    <row r="323" hidden="1" spans="1:12">
       <c r="A323">
         <v>322</v>
       </c>
@@ -26064,7 +26063,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="324" spans="1:11">
+    <row r="324" hidden="1" spans="1:11">
       <c r="A324">
         <v>323</v>
       </c>
@@ -26099,7 +26098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:11">
+    <row r="325" hidden="1" spans="1:11">
       <c r="A325">
         <v>324</v>
       </c>
@@ -26134,7 +26133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:12">
+    <row r="326" hidden="1" spans="1:12">
       <c r="A326">
         <v>325</v>
       </c>
@@ -26172,7 +26171,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="327" spans="1:11">
+    <row r="327" hidden="1" spans="1:11">
       <c r="A327">
         <v>326</v>
       </c>
@@ -26207,7 +26206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:11">
+    <row r="328" hidden="1" spans="1:11">
       <c r="A328">
         <v>327</v>
       </c>
@@ -26242,7 +26241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:12">
+    <row r="329" hidden="1" spans="1:12">
       <c r="A329">
         <v>328</v>
       </c>
@@ -26280,7 +26279,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="330" spans="1:12">
+    <row r="330" hidden="1" spans="1:12">
       <c r="A330">
         <v>329</v>
       </c>
@@ -26318,7 +26317,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="331" spans="1:12">
+    <row r="331" hidden="1" spans="1:12">
       <c r="A331">
         <v>330</v>
       </c>
@@ -26356,7 +26355,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="332" spans="1:12">
+    <row r="332" hidden="1" spans="1:12">
       <c r="A332">
         <v>331</v>
       </c>
@@ -26394,7 +26393,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="333" spans="1:11">
+    <row r="333" hidden="1" spans="1:11">
       <c r="A333">
         <v>332</v>
       </c>
@@ -26429,7 +26428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:12">
+    <row r="334" hidden="1" spans="1:12">
       <c r="A334">
         <v>333</v>
       </c>
@@ -26467,7 +26466,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="335" spans="1:12">
+    <row r="335" hidden="1" spans="1:12">
       <c r="A335">
         <v>334</v>
       </c>
@@ -26505,7 +26504,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="336" spans="1:12">
+    <row r="336" hidden="1" spans="1:12">
       <c r="A336">
         <v>335</v>
       </c>
@@ -26543,7 +26542,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="337" spans="1:11">
+    <row r="337" hidden="1" spans="1:11">
       <c r="A337">
         <v>336</v>
       </c>
@@ -26578,7 +26577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:12">
+    <row r="338" hidden="1" spans="1:12">
       <c r="A338">
         <v>337</v>
       </c>
@@ -26616,7 +26615,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="339" spans="1:12">
+    <row r="339" hidden="1" spans="1:12">
       <c r="A339">
         <v>338</v>
       </c>
@@ -26654,7 +26653,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="340" spans="1:12">
+    <row r="340" hidden="1" spans="1:12">
       <c r="A340">
         <v>339</v>
       </c>
@@ -26692,7 +26691,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="341" spans="1:12">
+    <row r="341" hidden="1" spans="1:12">
       <c r="A341">
         <v>340</v>
       </c>
@@ -26730,7 +26729,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="342" spans="1:11">
+    <row r="342" hidden="1" spans="1:11">
       <c r="A342">
         <v>341</v>
       </c>
@@ -26765,7 +26764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:12">
+    <row r="343" hidden="1" spans="1:12">
       <c r="A343">
         <v>342</v>
       </c>
@@ -26803,7 +26802,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="344" spans="1:11">
+    <row r="344" hidden="1" spans="1:11">
       <c r="A344">
         <v>343</v>
       </c>
@@ -26838,7 +26837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:12">
+    <row r="345" hidden="1" spans="1:12">
       <c r="A345">
         <v>344</v>
       </c>
@@ -26876,7 +26875,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="346" spans="1:11">
+    <row r="346" hidden="1" spans="1:11">
       <c r="A346">
         <v>345</v>
       </c>
@@ -26911,7 +26910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:11">
+    <row r="347" hidden="1" spans="1:11">
       <c r="A347">
         <v>346</v>
       </c>
@@ -26946,7 +26945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:12">
+    <row r="348" hidden="1" spans="1:12">
       <c r="A348">
         <v>347</v>
       </c>
@@ -26984,7 +26983,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="349" spans="1:11">
+    <row r="349" hidden="1" spans="1:11">
       <c r="A349">
         <v>348</v>
       </c>
@@ -27019,7 +27018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:11">
+    <row r="350" hidden="1" spans="1:11">
       <c r="A350">
         <v>349</v>
       </c>
@@ -27054,7 +27053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:12">
+    <row r="351" hidden="1" spans="1:12">
       <c r="A351">
         <v>350</v>
       </c>
@@ -27092,7 +27091,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="352" spans="1:11">
+    <row r="352" hidden="1" spans="1:11">
       <c r="A352">
         <v>351</v>
       </c>
@@ -27127,7 +27126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:12">
+    <row r="353" hidden="1" spans="1:12">
       <c r="A353">
         <v>352</v>
       </c>
@@ -27165,7 +27164,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="354" spans="1:11">
+    <row r="354" hidden="1" spans="1:11">
       <c r="A354">
         <v>353</v>
       </c>
@@ -27200,7 +27199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:12">
+    <row r="355" hidden="1" spans="1:12">
       <c r="A355">
         <v>354</v>
       </c>
@@ -27238,7 +27237,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="356" spans="1:11">
+    <row r="356" hidden="1" spans="1:11">
       <c r="A356">
         <v>355</v>
       </c>
@@ -27273,7 +27272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:12">
+    <row r="357" hidden="1" spans="1:12">
       <c r="A357">
         <v>356</v>
       </c>
@@ -27311,7 +27310,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="358" spans="1:12">
+    <row r="358" hidden="1" spans="1:12">
       <c r="A358">
         <v>357</v>
       </c>
@@ -27349,7 +27348,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="359" spans="1:11">
+    <row r="359" hidden="1" spans="1:11">
       <c r="A359">
         <v>358</v>
       </c>
@@ -27384,7 +27383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:11">
+    <row r="360" hidden="1" spans="1:11">
       <c r="A360">
         <v>359</v>
       </c>
@@ -27419,7 +27418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:12">
+    <row r="361" hidden="1" spans="1:12">
       <c r="A361">
         <v>360</v>
       </c>
@@ -27457,7 +27456,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="362" spans="1:11">
+    <row r="362" hidden="1" spans="1:11">
       <c r="A362">
         <v>361</v>
       </c>
@@ -27492,7 +27491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:11">
+    <row r="363" hidden="1" spans="1:11">
       <c r="A363">
         <v>362</v>
       </c>
@@ -27527,7 +27526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:11">
+    <row r="364" hidden="1" spans="1:11">
       <c r="A364">
         <v>363</v>
       </c>
@@ -27562,7 +27561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:11">
+    <row r="365" hidden="1" spans="1:11">
       <c r="A365">
         <v>364</v>
       </c>
@@ -27597,7 +27596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:11">
+    <row r="366" hidden="1" spans="1:11">
       <c r="A366">
         <v>365</v>
       </c>
@@ -27632,7 +27631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:12">
+    <row r="367" hidden="1" spans="1:12">
       <c r="A367">
         <v>366</v>
       </c>
@@ -27670,7 +27669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="368" spans="1:11">
+    <row r="368" hidden="1" spans="1:11">
       <c r="A368">
         <v>367</v>
       </c>
@@ -27705,7 +27704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:11">
+    <row r="369" hidden="1" spans="1:11">
       <c r="A369">
         <v>368</v>
       </c>
@@ -27740,7 +27739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:11">
+    <row r="370" hidden="1" spans="1:11">
       <c r="A370">
         <v>369</v>
       </c>
@@ -27775,7 +27774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:12">
+    <row r="371" hidden="1" spans="1:12">
       <c r="A371">
         <v>370</v>
       </c>
@@ -27813,7 +27812,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="372" spans="1:11">
+    <row r="372" hidden="1" spans="1:11">
       <c r="A372">
         <v>371</v>
       </c>
@@ -27848,7 +27847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:12">
+    <row r="373" hidden="1" spans="1:12">
       <c r="A373">
         <v>372</v>
       </c>
@@ -27886,7 +27885,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="374" spans="1:12">
+    <row r="374" hidden="1" spans="1:12">
       <c r="A374">
         <v>373</v>
       </c>
@@ -27924,7 +27923,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="375" spans="1:12">
+    <row r="375" hidden="1" spans="1:12">
       <c r="A375">
         <v>374</v>
       </c>
@@ -27962,7 +27961,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="376" spans="1:12">
+    <row r="376" hidden="1" spans="1:12">
       <c r="A376">
         <v>375</v>
       </c>
@@ -28000,7 +27999,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="377" spans="1:11">
+    <row r="377" hidden="1" spans="1:11">
       <c r="A377">
         <v>376</v>
       </c>
@@ -28035,7 +28034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:12">
+    <row r="378" hidden="1" spans="1:12">
       <c r="A378">
         <v>377</v>
       </c>
@@ -28073,7 +28072,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="379" spans="1:12">
+    <row r="379" hidden="1" spans="1:12">
       <c r="A379">
         <v>378</v>
       </c>
@@ -28111,7 +28110,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="380" spans="1:12">
+    <row r="380" hidden="1" spans="1:12">
       <c r="A380">
         <v>379</v>
       </c>
@@ -28149,7 +28148,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="381" spans="1:11">
+    <row r="381" hidden="1" spans="1:11">
       <c r="A381">
         <v>380</v>
       </c>
@@ -28184,7 +28183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:11">
+    <row r="382" hidden="1" spans="1:11">
       <c r="A382">
         <v>381</v>
       </c>
@@ -28219,7 +28218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:12">
+    <row r="383" hidden="1" spans="1:12">
       <c r="A383">
         <v>382</v>
       </c>
@@ -28257,7 +28256,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="384" spans="1:11">
+    <row r="384" hidden="1" spans="1:11">
       <c r="A384">
         <v>383</v>
       </c>
@@ -28292,7 +28291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:11">
+    <row r="385" hidden="1" spans="1:11">
       <c r="A385">
         <v>384</v>
       </c>
@@ -28327,7 +28326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:11">
+    <row r="386" hidden="1" spans="1:11">
       <c r="A386">
         <v>385</v>
       </c>
@@ -28362,7 +28361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:11">
+    <row r="387" hidden="1" spans="1:11">
       <c r="A387">
         <v>386</v>
       </c>
@@ -28397,7 +28396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:11">
+    <row r="388" hidden="1" spans="1:11">
       <c r="A388">
         <v>387</v>
       </c>
@@ -28432,7 +28431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:12">
+    <row r="389" hidden="1" spans="1:12">
       <c r="A389">
         <v>388</v>
       </c>
@@ -28470,7 +28469,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="390" spans="1:11">
+    <row r="390" hidden="1" spans="1:11">
       <c r="A390">
         <v>389</v>
       </c>
@@ -28505,7 +28504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:12">
+    <row r="391" hidden="1" spans="1:12">
       <c r="A391">
         <v>390</v>
       </c>
@@ -28543,7 +28542,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="392" spans="1:12">
+    <row r="392" hidden="1" spans="1:12">
       <c r="A392">
         <v>391</v>
       </c>
@@ -28581,7 +28580,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="393" spans="1:12">
+    <row r="393" hidden="1" spans="1:12">
       <c r="A393">
         <v>392</v>
       </c>
@@ -28619,7 +28618,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="394" spans="1:11">
+    <row r="394" hidden="1" spans="1:11">
       <c r="A394">
         <v>393</v>
       </c>
@@ -28654,7 +28653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:12">
+    <row r="395" hidden="1" spans="1:12">
       <c r="A395">
         <v>394</v>
       </c>
@@ -28692,7 +28691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="396" spans="1:12">
+    <row r="396" hidden="1" spans="1:12">
       <c r="A396">
         <v>395</v>
       </c>
@@ -28730,7 +28729,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="397" spans="1:11">
+    <row r="397" hidden="1" spans="1:11">
       <c r="A397">
         <v>396</v>
       </c>
@@ -28765,7 +28764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:11">
+    <row r="398" hidden="1" spans="1:11">
       <c r="A398">
         <v>397</v>
       </c>
@@ -28800,7 +28799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:11">
+    <row r="399" hidden="1" spans="1:11">
       <c r="A399">
         <v>398</v>
       </c>
@@ -28835,7 +28834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:12">
+    <row r="400" hidden="1" spans="1:12">
       <c r="A400">
         <v>399</v>
       </c>
@@ -28873,7 +28872,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="401" spans="1:11">
+    <row r="401" hidden="1" spans="1:11">
       <c r="A401">
         <v>400</v>
       </c>
@@ -28908,7 +28907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:11">
+    <row r="402" hidden="1" spans="1:11">
       <c r="A402">
         <v>401</v>
       </c>
@@ -28943,7 +28942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:11">
+    <row r="403" hidden="1" spans="1:11">
       <c r="A403">
         <v>402</v>
       </c>
@@ -28978,7 +28977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:11">
+    <row r="404" hidden="1" spans="1:11">
       <c r="A404">
         <v>403</v>
       </c>
@@ -29013,7 +29012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:11">
+    <row r="405" hidden="1" spans="1:11">
       <c r="A405">
         <v>404</v>
       </c>
@@ -29048,7 +29047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:11">
+    <row r="406" hidden="1" spans="1:11">
       <c r="A406">
         <v>405</v>
       </c>
@@ -29083,7 +29082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:11">
+    <row r="407" hidden="1" spans="1:11">
       <c r="A407">
         <v>406</v>
       </c>
@@ -29118,7 +29117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:12">
+    <row r="408" hidden="1" spans="1:12">
       <c r="A408">
         <v>407</v>
       </c>
@@ -29156,7 +29155,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="409" spans="1:12">
+    <row r="409" hidden="1" spans="1:12">
       <c r="A409">
         <v>408</v>
       </c>
@@ -29194,7 +29193,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="410" spans="1:12">
+    <row r="410" hidden="1" spans="1:12">
       <c r="A410">
         <v>409</v>
       </c>
@@ -29232,7 +29231,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="411" spans="1:11">
+    <row r="411" hidden="1" spans="1:11">
       <c r="A411">
         <v>410</v>
       </c>
@@ -29267,7 +29266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:12">
+    <row r="412" hidden="1" spans="1:12">
       <c r="A412">
         <v>411</v>
       </c>
@@ -29305,7 +29304,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="413" spans="1:11">
+    <row r="413" hidden="1" spans="1:11">
       <c r="A413">
         <v>412</v>
       </c>
@@ -29340,7 +29339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:12">
+    <row r="414" hidden="1" spans="1:12">
       <c r="A414">
         <v>413</v>
       </c>
@@ -29378,7 +29377,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="415" spans="1:12">
+    <row r="415" hidden="1" spans="1:12">
       <c r="A415">
         <v>414</v>
       </c>
@@ -29416,7 +29415,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="416" spans="1:12">
+    <row r="416" hidden="1" spans="1:12">
       <c r="A416">
         <v>415</v>
       </c>
@@ -29454,7 +29453,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="417" spans="1:11">
+    <row r="417" hidden="1" spans="1:11">
       <c r="A417">
         <v>416</v>
       </c>
@@ -29489,7 +29488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:11">
+    <row r="418" hidden="1" spans="1:11">
       <c r="A418">
         <v>417</v>
       </c>
@@ -29524,7 +29523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:12">
+    <row r="419" hidden="1" spans="1:12">
       <c r="A419">
         <v>418</v>
       </c>
@@ -29562,7 +29561,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="420" spans="1:11">
+    <row r="420" hidden="1" spans="1:11">
       <c r="A420">
         <v>419</v>
       </c>
@@ -29597,7 +29596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:11">
+    <row r="421" hidden="1" spans="1:11">
       <c r="A421">
         <v>420</v>
       </c>
@@ -29632,7 +29631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:11">
+    <row r="422" hidden="1" spans="1:11">
       <c r="A422">
         <v>421</v>
       </c>
@@ -29667,7 +29666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:11">
+    <row r="423" hidden="1" spans="1:11">
       <c r="A423">
         <v>422</v>
       </c>
@@ -29702,7 +29701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:11">
+    <row r="424" hidden="1" spans="1:11">
       <c r="A424">
         <v>423</v>
       </c>
@@ -29737,7 +29736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:11">
+    <row r="425" hidden="1" spans="1:11">
       <c r="A425">
         <v>424</v>
       </c>
@@ -29772,7 +29771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:11">
+    <row r="426" hidden="1" spans="1:11">
       <c r="A426">
         <v>425</v>
       </c>
@@ -29807,7 +29806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:12">
+    <row r="427" hidden="1" spans="1:12">
       <c r="A427">
         <v>426</v>
       </c>
@@ -29845,7 +29844,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="428" spans="1:12">
+    <row r="428" hidden="1" spans="1:12">
       <c r="A428">
         <v>427</v>
       </c>
@@ -29883,7 +29882,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="429" spans="1:11">
+    <row r="429" hidden="1" spans="1:11">
       <c r="A429">
         <v>428</v>
       </c>
@@ -29918,7 +29917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:12">
+    <row r="430" hidden="1" spans="1:12">
       <c r="A430">
         <v>429</v>
       </c>
@@ -38529,7 +38528,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="669" spans="1:12">
+    <row r="669" hidden="1" spans="1:12">
       <c r="A669">
         <v>668</v>
       </c>
@@ -38567,7 +38566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="670" spans="1:12">
+    <row r="670" hidden="1" spans="1:12">
       <c r="A670">
         <v>669</v>
       </c>
@@ -38605,7 +38604,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="671" spans="1:11">
+    <row r="671" hidden="1" spans="1:11">
       <c r="A671">
         <v>670</v>
       </c>
@@ -38640,7 +38639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="672" spans="1:12">
+    <row r="672" hidden="1" spans="1:12">
       <c r="A672">
         <v>671</v>
       </c>
@@ -38678,7 +38677,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="673" spans="1:12">
+    <row r="673" hidden="1" spans="1:12">
       <c r="A673">
         <v>672</v>
       </c>
@@ -38716,7 +38715,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="674" spans="1:11">
+    <row r="674" hidden="1" spans="1:11">
       <c r="A674">
         <v>673</v>
       </c>
@@ -38751,7 +38750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="675" spans="1:12">
+    <row r="675" hidden="1" spans="1:12">
       <c r="A675">
         <v>674</v>
       </c>
@@ -38789,7 +38788,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="676" spans="1:12">
+    <row r="676" hidden="1" spans="1:12">
       <c r="A676">
         <v>675</v>
       </c>
@@ -38827,7 +38826,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="677" spans="1:11">
+    <row r="677" hidden="1" spans="1:11">
       <c r="A677">
         <v>676</v>
       </c>
@@ -38862,7 +38861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="678" spans="1:12">
+    <row r="678" hidden="1" spans="1:12">
       <c r="A678">
         <v>677</v>
       </c>
@@ -38900,7 +38899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="679" spans="1:11">
+    <row r="679" hidden="1" spans="1:11">
       <c r="A679">
         <v>678</v>
       </c>
@@ -38935,7 +38934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="680" spans="1:11">
+    <row r="680" hidden="1" spans="1:11">
       <c r="A680">
         <v>679</v>
       </c>
@@ -38970,7 +38969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="681" spans="1:12">
+    <row r="681" hidden="1" spans="1:12">
       <c r="A681">
         <v>680</v>
       </c>
@@ -39008,7 +39007,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="682" spans="1:12">
+    <row r="682" hidden="1" spans="1:12">
       <c r="A682">
         <v>681</v>
       </c>
@@ -39046,7 +39045,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="683" spans="1:11">
+    <row r="683" hidden="1" spans="1:11">
       <c r="A683">
         <v>683</v>
       </c>
@@ -39081,7 +39080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="684" spans="1:11">
+    <row r="684" hidden="1" spans="1:11">
       <c r="A684">
         <v>684</v>
       </c>
@@ -39116,7 +39115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="685" spans="1:11">
+    <row r="685" hidden="1" spans="1:11">
       <c r="A685">
         <v>685</v>
       </c>
@@ -39151,7 +39150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="686" spans="1:12">
+    <row r="686" hidden="1" spans="1:12">
       <c r="A686">
         <v>686</v>
       </c>
@@ -39189,7 +39188,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="687" spans="1:11">
+    <row r="687" hidden="1" spans="1:11">
       <c r="A687">
         <v>687</v>
       </c>
@@ -39224,7 +39223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="688" spans="1:12">
+    <row r="688" hidden="1" spans="1:12">
       <c r="A688">
         <v>688</v>
       </c>
@@ -39268,19 +39267,19 @@
       </c>
       <c r="F689" s="3">
         <f>SUBTOTAL(103,Table1[Barcode])</f>
-        <v>687</v>
+        <v>347</v>
       </c>
       <c r="J689" s="5">
         <f>SUBTOTAL(109,Table1[LineTotal])</f>
-        <v>730404.67</v>
+        <v>317409.09</v>
       </c>
       <c r="K689" s="5">
         <f>SUBTOTAL(109,Table1[BillAmount])</f>
-        <v>730657</v>
+        <v>317164</v>
       </c>
       <c r="L689">
         <f>SUBTOTAL(103,Table1[PayMode])</f>
-        <v>376</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>